<commit_message>
Presentation Done,META DATA-{batch list} done
</commit_message>
<xml_diff>
--- a/EmployeeDetail.xlsx
+++ b/EmployeeDetail.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="182">
   <si>
     <t xml:space="preserve">empId</t>
   </si>
@@ -59,7 +59,7 @@
     <t xml:space="preserve">contact</t>
   </si>
   <si>
-    <t xml:space="preserve">department</t>
+    <t xml:space="preserve">deptId</t>
   </si>
   <si>
     <t xml:space="preserve">isTeaching</t>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t xml:space="preserve">patelparth.140410107075@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comp.Engg.</t>
   </si>
   <si>
     <t xml:space="preserve">-</t>
@@ -735,8 +732,8 @@
   </sheetPr>
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -881,41 +878,41 @@
       <c r="L2" s="3" t="n">
         <v>9574421069</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>34</v>
+      <c r="M2" s="6" t="n">
+        <v>4</v>
       </c>
       <c r="N2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="0" t="s">
+      <c r="R2" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="S2" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="0" t="s">
+      <c r="T2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="T2" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="U2" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="V2" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -927,7 +924,7 @@
         <v>Ms.</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>26</v>
@@ -939,58 +936,58 @@
         <v>28</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="I3" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L3" s="3" t="n">
         <v>8511185939</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>34</v>
+      <c r="M3" s="6" t="n">
+        <v>4</v>
       </c>
       <c r="N3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="R3" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="S3" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S3" s="0" t="s">
+      <c r="T3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="U3" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="T3" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="U3" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="V3" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Y3" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1002,10 +999,10 @@
         <v>Ms.</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>46</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>27</v>
@@ -1014,58 +1011,58 @@
         <v>28</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>32</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L4" s="3" t="n">
         <v>8469582199</v>
       </c>
-      <c r="M4" s="6" t="s">
-        <v>34</v>
+      <c r="M4" s="6" t="n">
+        <v>4</v>
       </c>
       <c r="N4" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q4" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="R4" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="R4" s="0" t="s">
+      <c r="S4" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S4" s="0" t="s">
+      <c r="T4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="U4" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="T4" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="U4" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="V4" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W4" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Y4" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1077,10 +1074,10 @@
         <v>Mr.</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>51</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>27</v>
@@ -1089,58 +1086,58 @@
         <v>28</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H5" s="0" t="s">
         <v>30</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>32</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L5" s="3" t="n">
         <v>9426625662</v>
       </c>
-      <c r="M5" s="6" t="s">
-        <v>34</v>
+      <c r="M5" s="6" t="n">
+        <v>4</v>
       </c>
       <c r="N5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="Q5" s="0" t="s">
+      <c r="R5" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="R5" s="0" t="s">
+      <c r="S5" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S5" s="0" t="s">
+      <c r="T5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="T5" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="U5" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="V5" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W5" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="X5" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Y5" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1152,10 +1149,10 @@
         <v>Ms.</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>27</v>
@@ -1164,58 +1161,58 @@
         <v>28</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="H6" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>32</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L6" s="3" t="n">
         <v>7041606679</v>
       </c>
-      <c r="M6" s="6" t="s">
-        <v>34</v>
+      <c r="M6" s="6" t="n">
+        <v>4</v>
       </c>
       <c r="N6" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="Q6" s="0" t="s">
+      <c r="R6" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="R6" s="0" t="s">
+      <c r="S6" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S6" s="0" t="s">
+      <c r="T6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="U6" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="T6" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="U6" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="V6" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W6" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Y6" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1227,10 +1224,10 @@
         <v>Ms.</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>27</v>
@@ -1239,58 +1236,58 @@
         <v>28</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>32</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L7" s="3" t="n">
         <v>7046449857</v>
       </c>
-      <c r="M7" s="6" t="s">
-        <v>34</v>
+      <c r="M7" s="6" t="n">
+        <v>7</v>
       </c>
       <c r="N7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q7" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="R7" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="R7" s="0" t="s">
+      <c r="S7" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S7" s="0" t="s">
+      <c r="T7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="U7" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="T7" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="U7" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="V7" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W7" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="X7" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Y7" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1302,10 +1299,10 @@
         <v>Mr.</v>
       </c>
       <c r="C8" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>64</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>27</v>
@@ -1314,58 +1311,58 @@
         <v>28</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H8" s="0" t="s">
         <v>30</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J8" s="5" t="s">
         <v>32</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L8" s="3" t="n">
         <v>7622815525</v>
       </c>
-      <c r="M8" s="6" t="s">
-        <v>34</v>
+      <c r="M8" s="6" t="n">
+        <v>7</v>
       </c>
       <c r="N8" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q8" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="Q8" s="0" t="s">
+      <c r="R8" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="R8" s="0" t="s">
+      <c r="S8" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S8" s="0" t="s">
+      <c r="T8" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="U8" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="T8" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="U8" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="V8" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W8" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="X8" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Y8" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1377,10 +1374,10 @@
         <v>Mr.</v>
       </c>
       <c r="C9" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>69</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>27</v>
@@ -1389,58 +1386,58 @@
         <v>28</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>30</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>32</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L9" s="3" t="n">
         <v>8128983156</v>
       </c>
-      <c r="M9" s="6" t="s">
-        <v>34</v>
+      <c r="M9" s="6" t="n">
+        <v>7</v>
       </c>
       <c r="N9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q9" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="Q9" s="0" t="s">
+      <c r="R9" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="R9" s="0" t="s">
+      <c r="S9" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S9" s="0" t="s">
+      <c r="T9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="U9" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="T9" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="U9" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="V9" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W9" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="X9" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Y9" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1452,70 +1449,70 @@
         <v>Ms.</v>
       </c>
       <c r="C10" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="E10" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>77</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>32</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L10" s="3" t="n">
         <v>9428200189</v>
       </c>
-      <c r="M10" s="6" t="s">
-        <v>34</v>
+      <c r="M10" s="6" t="n">
+        <v>7</v>
       </c>
       <c r="N10" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q10" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="Q10" s="0" t="s">
+      <c r="R10" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="R10" s="0" t="s">
+      <c r="S10" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S10" s="0" t="s">
+      <c r="T10" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="U10" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="T10" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="U10" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="V10" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W10" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="X10" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Y10" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1527,70 +1524,70 @@
         <v>Ms.</v>
       </c>
       <c r="C11" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>80</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>32</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L11" s="3" t="n">
         <v>9173616991</v>
       </c>
-      <c r="M11" s="6" t="s">
-        <v>34</v>
+      <c r="M11" s="6" t="n">
+        <v>7</v>
       </c>
       <c r="N11" s="0" t="n">
         <v>1</v>
       </c>
       <c r="P11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q11" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="Q11" s="0" t="s">
+      <c r="R11" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="R11" s="0" t="s">
+      <c r="S11" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="S11" s="0" t="s">
+      <c r="T11" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="U11" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="T11" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="U11" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="V11" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="X11" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Y11" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1641,7 +1638,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>26</v>
@@ -1652,10 +1649,10 @@
         <v>27</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1663,10 +1660,10 @@
         <v>27</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1674,10 +1671,10 @@
         <v>27</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1685,10 +1682,10 @@
         <v>27</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1696,10 +1693,10 @@
         <v>27</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>63</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1707,62 +1704,62 @@
         <v>27</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>73</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>26</v>
@@ -1770,175 +1767,175 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>90</v>
-      </c>
       <c r="C15" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="C16" s="0" t="s">
         <v>92</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="C17" s="0" t="s">
         <v>95</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="C18" s="0" t="s">
         <v>98</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>101</v>
-      </c>
       <c r="C19" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="C20" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>106</v>
-      </c>
       <c r="C21" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="C22" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="B23" s="0" t="s">
-        <v>111</v>
-      </c>
       <c r="C23" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="B24" s="0" t="s">
-        <v>113</v>
-      </c>
       <c r="C24" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="0" t="s">
         <v>115</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>26</v>
@@ -1946,90 +1943,90 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B33" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" s="0" t="s">
         <v>123</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2037,131 +2034,131 @@
         <v>27</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B39" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="B39" s="0" t="s">
-        <v>130</v>
-      </c>
       <c r="C39" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B41" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="B41" s="0" t="s">
-        <v>133</v>
-      </c>
       <c r="C41" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B42" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="B42" s="0" t="s">
-        <v>135</v>
-      </c>
       <c r="C42" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B43" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="B43" s="0" t="s">
-        <v>137</v>
-      </c>
       <c r="C43" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B44" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="B44" s="0" t="s">
-        <v>139</v>
-      </c>
       <c r="C44" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B45" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="B45" s="0" t="s">
-        <v>141</v>
-      </c>
       <c r="C45" s="0" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B46" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="B46" s="0" t="s">
-        <v>143</v>
-      </c>
       <c r="C46" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B47" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="B47" s="0" t="s">
-        <v>145</v>
-      </c>
       <c r="C47" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B48" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="B48" s="0" t="s">
-        <v>147</v>
-      </c>
       <c r="C48" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B49" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="B49" s="0" t="s">
-        <v>149</v>
-      </c>
       <c r="C49" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2169,200 +2166,200 @@
         <v>27</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B51" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="C51" s="0" t="s">
         <v>152</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B52" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="C52" s="0" t="s">
         <v>155</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B53" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="C53" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="D53" s="0" t="s">
         <v>159</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="B55" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="B55" s="0" t="s">
-        <v>163</v>
-      </c>
       <c r="C55" s="0" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B57" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="B57" s="0" t="s">
-        <v>166</v>
-      </c>
       <c r="C57" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B58" s="0" t="s">
         <v>167</v>
       </c>
-      <c r="B58" s="0" t="s">
-        <v>168</v>
-      </c>
       <c r="C58" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B60" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C60" s="0" t="s">
         <v>170</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="B64" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="B64" s="0" t="s">
-        <v>176</v>
-      </c>
       <c r="C64" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B65" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="B65" s="0" t="s">
-        <v>178</v>
-      </c>
       <c r="C65" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B66" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="B66" s="0" t="s">
-        <v>180</v>
-      </c>
       <c r="C66" s="0" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B67" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="B67" s="0" t="s">
-        <v>182</v>
-      </c>
       <c r="C67" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>